<commit_message>
Agregado parametro para ejecutar query
</commit_message>
<xml_diff>
--- a/MANTENER TABLAS DATOS.xlsx
+++ b/MANTENER TABLAS DATOS.xlsx
@@ -2636,7 +2636,7 @@
     <t>PAC_USUARIO_MAE</t>
   </si>
   <si>
-    <t>PRESTAMOCUOTAFECHA</t>
+    <t>PRESTAMOCUOTASFECHA</t>
   </si>
 </sst>
 </file>
@@ -8321,7 +8321,7 @@
         <v>4</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>483</v>
+        <v>869</v>
       </c>
       <c r="C486" t="s">
         <v>863</v>
@@ -8332,7 +8332,7 @@
         <v>4</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C487" t="s">
         <v>863</v>
@@ -8343,7 +8343,7 @@
         <v>4</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C488" t="s">
         <v>863</v>
@@ -8354,7 +8354,7 @@
         <v>4</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C489" t="s">
         <v>863</v>
@@ -8365,7 +8365,7 @@
         <v>4</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C490" t="s">
         <v>863</v>
@@ -8376,7 +8376,7 @@
         <v>4</v>
       </c>
       <c r="B491" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C491" t="s">
         <v>863</v>
@@ -8387,7 +8387,7 @@
         <v>4</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C492" t="s">
         <v>863</v>
@@ -8398,7 +8398,7 @@
         <v>4</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C493" t="s">
         <v>863</v>
@@ -8409,7 +8409,7 @@
         <v>4</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C494" t="s">
         <v>863</v>
@@ -8420,7 +8420,7 @@
         <v>4</v>
       </c>
       <c r="B495" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C495" t="s">
         <v>863</v>
@@ -8431,7 +8431,7 @@
         <v>4</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C496" t="s">
         <v>863</v>
@@ -8442,7 +8442,7 @@
         <v>4</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C497" t="s">
         <v>863</v>
@@ -8453,7 +8453,7 @@
         <v>4</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C498" t="s">
         <v>863</v>
@@ -8464,7 +8464,7 @@
         <v>4</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C499" t="s">
         <v>863</v>
@@ -8475,7 +8475,7 @@
         <v>4</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C500" t="s">
         <v>863</v>
@@ -8486,7 +8486,7 @@
         <v>4</v>
       </c>
       <c r="B501" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C501" t="s">
         <v>863</v>
@@ -8497,7 +8497,7 @@
         <v>4</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C502" t="s">
         <v>863</v>
@@ -8508,7 +8508,7 @@
         <v>4</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C503" t="s">
         <v>863</v>
@@ -8519,7 +8519,7 @@
         <v>4</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C504" t="s">
         <v>863</v>
@@ -8530,7 +8530,7 @@
         <v>4</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C505" t="s">
         <v>863</v>
@@ -8541,7 +8541,7 @@
         <v>4</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C506" t="s">
         <v>863</v>
@@ -8552,7 +8552,7 @@
         <v>4</v>
       </c>
       <c r="B507" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C507" t="s">
         <v>863</v>
@@ -8563,7 +8563,7 @@
         <v>4</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C508" t="s">
         <v>863</v>
@@ -8574,7 +8574,7 @@
         <v>4</v>
       </c>
       <c r="B509" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C509" t="s">
         <v>863</v>
@@ -8585,7 +8585,7 @@
         <v>4</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C510" t="s">
         <v>863</v>
@@ -8596,7 +8596,7 @@
         <v>4</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C511" t="s">
         <v>863</v>
@@ -8607,7 +8607,7 @@
         <v>4</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C512" t="s">
         <v>863</v>
@@ -8618,7 +8618,7 @@
         <v>4</v>
       </c>
       <c r="B513" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C513" t="s">
         <v>863</v>
@@ -8629,7 +8629,7 @@
         <v>4</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C514" t="s">
         <v>863</v>
@@ -8640,7 +8640,7 @@
         <v>4</v>
       </c>
       <c r="B515" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C515" t="s">
         <v>863</v>
@@ -8651,7 +8651,7 @@
         <v>4</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C516" t="s">
         <v>863</v>
@@ -8662,7 +8662,7 @@
         <v>4</v>
       </c>
       <c r="B517" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C517" t="s">
         <v>863</v>
@@ -8673,7 +8673,7 @@
         <v>4</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C518" t="s">
         <v>863</v>
@@ -8684,7 +8684,7 @@
         <v>4</v>
       </c>
       <c r="B519" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C519" t="s">
         <v>863</v>
@@ -8695,7 +8695,7 @@
         <v>4</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C520" t="s">
         <v>863</v>
@@ -8706,7 +8706,7 @@
         <v>4</v>
       </c>
       <c r="B521" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C521" t="s">
         <v>863</v>
@@ -8717,7 +8717,7 @@
         <v>4</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C522" t="s">
         <v>863</v>
@@ -8728,7 +8728,7 @@
         <v>4</v>
       </c>
       <c r="B523" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C523" t="s">
         <v>863</v>
@@ -8739,7 +8739,7 @@
         <v>4</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C524" t="s">
         <v>863</v>
@@ -8750,7 +8750,7 @@
         <v>4</v>
       </c>
       <c r="B525" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C525" t="s">
         <v>863</v>
@@ -8761,7 +8761,7 @@
         <v>4</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C526" t="s">
         <v>863</v>
@@ -8772,7 +8772,7 @@
         <v>4</v>
       </c>
       <c r="B527" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C527" t="s">
         <v>863</v>
@@ -8783,7 +8783,7 @@
         <v>4</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C528" t="s">
         <v>863</v>
@@ -8794,7 +8794,7 @@
         <v>4</v>
       </c>
       <c r="B529" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C529" t="s">
         <v>863</v>
@@ -8805,7 +8805,7 @@
         <v>4</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C530" t="s">
         <v>863</v>
@@ -8816,7 +8816,7 @@
         <v>4</v>
       </c>
       <c r="B531" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C531" t="s">
         <v>863</v>
@@ -8827,7 +8827,7 @@
         <v>4</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C532" t="s">
         <v>863</v>
@@ -8838,7 +8838,7 @@
         <v>4</v>
       </c>
       <c r="B533" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C533" t="s">
         <v>863</v>
@@ -8849,7 +8849,7 @@
         <v>4</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C534" t="s">
         <v>863</v>
@@ -8860,7 +8860,7 @@
         <v>4</v>
       </c>
       <c r="B535" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C535" t="s">
         <v>863</v>
@@ -8871,7 +8871,7 @@
         <v>4</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C536" t="s">
         <v>863</v>
@@ -8882,7 +8882,7 @@
         <v>4</v>
       </c>
       <c r="B537" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C537" t="s">
         <v>863</v>
@@ -8893,7 +8893,7 @@
         <v>4</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C538" t="s">
         <v>863</v>
@@ -8904,7 +8904,7 @@
         <v>4</v>
       </c>
       <c r="B539" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C539" t="s">
         <v>863</v>
@@ -8915,7 +8915,7 @@
         <v>4</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C540" t="s">
         <v>863</v>
@@ -8926,7 +8926,7 @@
         <v>4</v>
       </c>
       <c r="B541" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C541" t="s">
         <v>863</v>
@@ -8937,7 +8937,7 @@
         <v>4</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C542" t="s">
         <v>863</v>
@@ -8948,7 +8948,7 @@
         <v>4</v>
       </c>
       <c r="B543" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C543" t="s">
         <v>863</v>
@@ -8959,7 +8959,7 @@
         <v>4</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C544" t="s">
         <v>863</v>
@@ -8970,7 +8970,7 @@
         <v>4</v>
       </c>
       <c r="B545" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C545" t="s">
         <v>863</v>
@@ -8981,7 +8981,7 @@
         <v>4</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C546" t="s">
         <v>863</v>
@@ -8992,7 +8992,7 @@
         <v>4</v>
       </c>
       <c r="B547" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C547" t="s">
         <v>863</v>
@@ -9003,7 +9003,7 @@
         <v>4</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C548" t="s">
         <v>863</v>
@@ -9014,7 +9014,7 @@
         <v>4</v>
       </c>
       <c r="B549" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C549" t="s">
         <v>863</v>
@@ -9025,7 +9025,7 @@
         <v>4</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C550" t="s">
         <v>863</v>
@@ -9036,7 +9036,7 @@
         <v>4</v>
       </c>
       <c r="B551" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C551" t="s">
         <v>863</v>
@@ -9047,7 +9047,7 @@
         <v>4</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C552" t="s">
         <v>863</v>
@@ -9058,7 +9058,7 @@
         <v>4</v>
       </c>
       <c r="B553" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C553" t="s">
         <v>863</v>
@@ -9069,7 +9069,7 @@
         <v>4</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C554" t="s">
         <v>863</v>
@@ -9080,7 +9080,7 @@
         <v>4</v>
       </c>
       <c r="B555" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C555" t="s">
         <v>863</v>
@@ -9091,7 +9091,7 @@
         <v>4</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C556" t="s">
         <v>863</v>
@@ -9102,7 +9102,7 @@
         <v>4</v>
       </c>
       <c r="B557" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C557" t="s">
         <v>863</v>
@@ -9113,7 +9113,7 @@
         <v>4</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C558" t="s">
         <v>863</v>
@@ -9124,7 +9124,7 @@
         <v>4</v>
       </c>
       <c r="B559" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C559" t="s">
         <v>863</v>
@@ -9135,7 +9135,7 @@
         <v>4</v>
       </c>
       <c r="B560" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C560" t="s">
         <v>863</v>
@@ -9146,7 +9146,7 @@
         <v>4</v>
       </c>
       <c r="B561" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C561" t="s">
         <v>863</v>
@@ -9157,7 +9157,7 @@
         <v>4</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C562" t="s">
         <v>863</v>
@@ -9168,7 +9168,7 @@
         <v>4</v>
       </c>
       <c r="B563" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C563" t="s">
         <v>863</v>
@@ -9179,7 +9179,7 @@
         <v>4</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C564" t="s">
         <v>863</v>
@@ -9190,7 +9190,7 @@
         <v>4</v>
       </c>
       <c r="B565" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C565" t="s">
         <v>863</v>
@@ -9201,7 +9201,7 @@
         <v>4</v>
       </c>
       <c r="B566" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C566" t="s">
         <v>863</v>
@@ -9212,7 +9212,7 @@
         <v>4</v>
       </c>
       <c r="B567" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C567" t="s">
         <v>863</v>
@@ -9223,7 +9223,7 @@
         <v>4</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C568" t="s">
         <v>863</v>
@@ -9234,7 +9234,7 @@
         <v>4</v>
       </c>
       <c r="B569" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C569" t="s">
         <v>863</v>
@@ -9245,7 +9245,7 @@
         <v>4</v>
       </c>
       <c r="B570" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C570" t="s">
         <v>863</v>
@@ -9256,7 +9256,7 @@
         <v>4</v>
       </c>
       <c r="B571" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C571" t="s">
         <v>863</v>
@@ -9267,7 +9267,7 @@
         <v>4</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C572" t="s">
         <v>863</v>
@@ -9278,7 +9278,7 @@
         <v>4</v>
       </c>
       <c r="B573" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C573" t="s">
         <v>863</v>
@@ -9289,7 +9289,7 @@
         <v>4</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C574" t="s">
         <v>863</v>
@@ -9300,7 +9300,7 @@
         <v>4</v>
       </c>
       <c r="B575" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C575" t="s">
         <v>863</v>
@@ -9311,7 +9311,7 @@
         <v>4</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C576" t="s">
         <v>863</v>
@@ -9322,7 +9322,7 @@
         <v>4</v>
       </c>
       <c r="B577" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C577" t="s">
         <v>863</v>
@@ -9333,7 +9333,7 @@
         <v>4</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C578" t="s">
         <v>863</v>
@@ -9344,7 +9344,7 @@
         <v>4</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C579" t="s">
         <v>863</v>
@@ -9355,7 +9355,7 @@
         <v>4</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C580" t="s">
         <v>863</v>
@@ -9366,7 +9366,7 @@
         <v>4</v>
       </c>
       <c r="B581" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C581" t="s">
         <v>863</v>
@@ -9377,7 +9377,7 @@
         <v>4</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C582" t="s">
         <v>863</v>
@@ -9388,7 +9388,7 @@
         <v>4</v>
       </c>
       <c r="B583" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C583" t="s">
         <v>863</v>
@@ -9399,7 +9399,7 @@
         <v>4</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C584" t="s">
         <v>863</v>
@@ -9410,7 +9410,7 @@
         <v>4</v>
       </c>
       <c r="B585" s="2" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="C585" t="s">
         <v>863</v>
@@ -9421,7 +9421,7 @@
         <v>4</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="C586" t="s">
         <v>863</v>
@@ -9432,7 +9432,7 @@
         <v>4</v>
       </c>
       <c r="B587" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C587" t="s">
         <v>863</v>
@@ -9443,7 +9443,7 @@
         <v>4</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C588" t="s">
         <v>863</v>
@@ -9454,7 +9454,7 @@
         <v>4</v>
       </c>
       <c r="B589" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C589" t="s">
         <v>863</v>
@@ -9465,7 +9465,7 @@
         <v>4</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C590" t="s">
         <v>863</v>
@@ -9476,7 +9476,7 @@
         <v>4</v>
       </c>
       <c r="B591" s="2" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="C591" t="s">
         <v>863</v>
@@ -9487,7 +9487,7 @@
         <v>4</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>588</v>
+        <v>599</v>
       </c>
       <c r="C592" t="s">
         <v>863</v>
@@ -9498,7 +9498,7 @@
         <v>4</v>
       </c>
       <c r="B593" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C593" t="s">
         <v>863</v>
@@ -9509,7 +9509,7 @@
         <v>4</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C594" t="s">
         <v>863</v>
@@ -9520,7 +9520,7 @@
         <v>4</v>
       </c>
       <c r="B595" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C595" t="s">
         <v>863</v>
@@ -9531,7 +9531,7 @@
         <v>4</v>
       </c>
       <c r="B596" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C596" t="s">
         <v>863</v>
@@ -9542,7 +9542,7 @@
         <v>4</v>
       </c>
       <c r="B597" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C597" t="s">
         <v>863</v>
@@ -9553,7 +9553,7 @@
         <v>4</v>
       </c>
       <c r="B598" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C598" t="s">
         <v>863</v>
@@ -9564,7 +9564,7 @@
         <v>4</v>
       </c>
       <c r="B599" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C599" t="s">
         <v>863</v>
@@ -9575,7 +9575,7 @@
         <v>4</v>
       </c>
       <c r="B600" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C600" t="s">
         <v>863</v>
@@ -9586,7 +9586,7 @@
         <v>4</v>
       </c>
       <c r="B601" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C601" t="s">
         <v>863</v>
@@ -9597,7 +9597,7 @@
         <v>4</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C602" t="s">
         <v>863</v>
@@ -9608,7 +9608,7 @@
         <v>4</v>
       </c>
       <c r="B603" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C603" t="s">
         <v>863</v>
@@ -9619,7 +9619,7 @@
         <v>4</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C604" t="s">
         <v>863</v>
@@ -9630,7 +9630,7 @@
         <v>4</v>
       </c>
       <c r="B605" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C605" t="s">
         <v>863</v>
@@ -9641,7 +9641,7 @@
         <v>4</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C606" t="s">
         <v>863</v>
@@ -9652,7 +9652,7 @@
         <v>4</v>
       </c>
       <c r="B607" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C607" t="s">
         <v>863</v>
@@ -9663,7 +9663,7 @@
         <v>4</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C608" t="s">
         <v>863</v>
@@ -9674,7 +9674,7 @@
         <v>4</v>
       </c>
       <c r="B609" s="2" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C609" t="s">
         <v>863</v>
@@ -9685,7 +9685,7 @@
         <v>4</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C610" t="s">
         <v>863</v>
@@ -9696,7 +9696,7 @@
         <v>4</v>
       </c>
       <c r="B611" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C611" t="s">
         <v>863</v>
@@ -9707,7 +9707,7 @@
         <v>4</v>
       </c>
       <c r="B612" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C612" t="s">
         <v>863</v>
@@ -9718,7 +9718,7 @@
         <v>4</v>
       </c>
       <c r="B613" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C613" t="s">
         <v>863</v>
@@ -9729,7 +9729,7 @@
         <v>4</v>
       </c>
       <c r="B614" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C614" t="s">
         <v>863</v>
@@ -9740,7 +9740,7 @@
         <v>4</v>
       </c>
       <c r="B615" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C615" t="s">
         <v>863</v>
@@ -9751,7 +9751,7 @@
         <v>4</v>
       </c>
       <c r="B616" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C616" t="s">
         <v>863</v>
@@ -9762,7 +9762,7 @@
         <v>4</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="C617" t="s">
         <v>863</v>
@@ -9773,7 +9773,7 @@
         <v>4</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="C618" t="s">
         <v>863</v>
@@ -9784,7 +9784,7 @@
         <v>4</v>
       </c>
       <c r="B619" s="2" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="C619" t="s">
         <v>863</v>
@@ -9795,7 +9795,7 @@
         <v>4</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C620" t="s">
         <v>863</v>
@@ -9806,7 +9806,7 @@
         <v>4</v>
       </c>
       <c r="B621" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C621" t="s">
         <v>863</v>
@@ -9817,7 +9817,7 @@
         <v>4</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C622" t="s">
         <v>863</v>
@@ -9828,7 +9828,7 @@
         <v>4</v>
       </c>
       <c r="B623" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C623" t="s">
         <v>863</v>
@@ -9839,7 +9839,7 @@
         <v>4</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C624" t="s">
         <v>863</v>
@@ -9850,7 +9850,7 @@
         <v>4</v>
       </c>
       <c r="B625" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C625" t="s">
         <v>863</v>
@@ -9861,7 +9861,7 @@
         <v>4</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="C626" t="s">
         <v>863</v>
@@ -9872,7 +9872,7 @@
         <v>4</v>
       </c>
       <c r="B627" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C627" t="s">
         <v>863</v>
@@ -9883,7 +9883,7 @@
         <v>4</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C628" t="s">
         <v>863</v>
@@ -9894,7 +9894,7 @@
         <v>4</v>
       </c>
       <c r="B629" s="2" t="s">
-        <v>653</v>
+        <v>626</v>
       </c>
       <c r="C629" t="s">
         <v>863</v>
@@ -9905,7 +9905,7 @@
         <v>4</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C630" t="s">
         <v>863</v>
@@ -9916,7 +9916,7 @@
         <v>4</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C631" t="s">
         <v>863</v>
@@ -9927,7 +9927,7 @@
         <v>4</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C632" t="s">
         <v>863</v>
@@ -9938,7 +9938,7 @@
         <v>4</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C633" t="s">
         <v>863</v>
@@ -9949,7 +9949,7 @@
         <v>4</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C634" t="s">
         <v>863</v>
@@ -9960,7 +9960,7 @@
         <v>4</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C635" t="s">
         <v>863</v>
@@ -9971,7 +9971,7 @@
         <v>4</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C636" t="s">
         <v>863</v>
@@ -9982,7 +9982,7 @@
         <v>4</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C637" t="s">
         <v>863</v>
@@ -9993,7 +9993,7 @@
         <v>4</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C638" t="s">
         <v>863</v>
@@ -10004,7 +10004,7 @@
         <v>4</v>
       </c>
       <c r="B639" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C639" t="s">
         <v>863</v>
@@ -10015,7 +10015,7 @@
         <v>4</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="C640" t="s">
         <v>863</v>
@@ -10026,7 +10026,7 @@
         <v>4</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C641" t="s">
         <v>863</v>
@@ -10037,7 +10037,7 @@
         <v>4</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C642" t="s">
         <v>863</v>
@@ -10048,7 +10048,7 @@
         <v>4</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C643" t="s">
         <v>863</v>
@@ -10059,7 +10059,7 @@
         <v>4</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="C644" t="s">
         <v>863</v>
@@ -10070,7 +10070,7 @@
         <v>4</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C645" t="s">
         <v>863</v>
@@ -10081,7 +10081,7 @@
         <v>4</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C646" t="s">
         <v>863</v>
@@ -10092,7 +10092,7 @@
         <v>4</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C647" t="s">
         <v>863</v>
@@ -10103,7 +10103,7 @@
         <v>4</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>627</v>
+        <v>667</v>
       </c>
       <c r="C648" t="s">
         <v>863</v>
@@ -10114,7 +10114,7 @@
         <v>4</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C649" t="s">
         <v>863</v>
@@ -10125,7 +10125,7 @@
         <v>4</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C650" t="s">
         <v>863</v>
@@ -10136,7 +10136,7 @@
         <v>4</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C651" t="s">
         <v>863</v>
@@ -10147,7 +10147,7 @@
         <v>4</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C652" t="s">
         <v>863</v>
@@ -10158,7 +10158,7 @@
         <v>4</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C653" t="s">
         <v>863</v>
@@ -10169,7 +10169,7 @@
         <v>4</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C654" t="s">
         <v>863</v>
@@ -10180,7 +10180,7 @@
         <v>4</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C655" t="s">
         <v>863</v>
@@ -10191,7 +10191,7 @@
         <v>4</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C656" t="s">
         <v>863</v>
@@ -10202,7 +10202,7 @@
         <v>4</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C657" t="s">
         <v>863</v>
@@ -10213,7 +10213,7 @@
         <v>4</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C658" t="s">
         <v>863</v>
@@ -10224,7 +10224,7 @@
         <v>4</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C659" t="s">
         <v>863</v>
@@ -10235,7 +10235,7 @@
         <v>4</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C660" t="s">
         <v>863</v>
@@ -10246,7 +10246,7 @@
         <v>4</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C661" t="s">
         <v>863</v>
@@ -10257,7 +10257,7 @@
         <v>4</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C662" t="s">
         <v>863</v>
@@ -10268,7 +10268,7 @@
         <v>4</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C663" t="s">
         <v>863</v>
@@ -10279,7 +10279,7 @@
         <v>4</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C664" t="s">
         <v>863</v>
@@ -10290,7 +10290,7 @@
         <v>4</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C665" t="s">
         <v>863</v>
@@ -10301,7 +10301,7 @@
         <v>4</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C666" t="s">
         <v>863</v>
@@ -10312,7 +10312,7 @@
         <v>4</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C667" t="s">
         <v>863</v>
@@ -10323,7 +10323,7 @@
         <v>4</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C668" t="s">
         <v>863</v>
@@ -10334,7 +10334,7 @@
         <v>4</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C669" t="s">
         <v>863</v>
@@ -10345,7 +10345,7 @@
         <v>4</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C670" t="s">
         <v>863</v>
@@ -10356,7 +10356,7 @@
         <v>4</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C671" t="s">
         <v>863</v>
@@ -10367,7 +10367,7 @@
         <v>4</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C672" t="s">
         <v>863</v>
@@ -10378,7 +10378,7 @@
         <v>4</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C673" t="s">
         <v>863</v>
@@ -10389,7 +10389,7 @@
         <v>4</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>672</v>
+        <v>652</v>
       </c>
       <c r="C674" t="s">
         <v>863</v>
@@ -10400,7 +10400,7 @@
         <v>4</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C675" t="s">
         <v>863</v>
@@ -10411,7 +10411,7 @@
         <v>4</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C676" t="s">
         <v>863</v>
@@ -10422,7 +10422,7 @@
         <v>4</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C677" t="s">
         <v>863</v>
@@ -10433,7 +10433,7 @@
         <v>4</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C678" t="s">
         <v>863</v>
@@ -10444,7 +10444,7 @@
         <v>4</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C679" t="s">
         <v>863</v>
@@ -10455,7 +10455,7 @@
         <v>4</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C680" t="s">
         <v>863</v>
@@ -10466,7 +10466,7 @@
         <v>4</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C681" t="s">
         <v>863</v>
@@ -10477,7 +10477,7 @@
         <v>4</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C682" t="s">
         <v>863</v>
@@ -10488,7 +10488,7 @@
         <v>4</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C683" t="s">
         <v>863</v>
@@ -10499,7 +10499,7 @@
         <v>4</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C684" t="s">
         <v>863</v>
@@ -10510,7 +10510,7 @@
         <v>4</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C685" t="s">
         <v>863</v>
@@ -10521,7 +10521,7 @@
         <v>4</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C686" t="s">
         <v>863</v>
@@ -10532,7 +10532,7 @@
         <v>4</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C687" t="s">
         <v>863</v>
@@ -10543,7 +10543,7 @@
         <v>4</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C688" t="s">
         <v>863</v>
@@ -10554,7 +10554,7 @@
         <v>4</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C689" t="s">
         <v>863</v>
@@ -10565,7 +10565,7 @@
         <v>4</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C690" t="s">
         <v>863</v>
@@ -10576,7 +10576,7 @@
         <v>4</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C691" t="s">
         <v>863</v>
@@ -10587,7 +10587,7 @@
         <v>4</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C692" t="s">
         <v>863</v>
@@ -10598,7 +10598,7 @@
         <v>4</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C693" t="s">
         <v>863</v>
@@ -10609,7 +10609,7 @@
         <v>4</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C694" t="s">
         <v>863</v>
@@ -10620,7 +10620,7 @@
         <v>4</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C695" t="s">
         <v>863</v>
@@ -10631,7 +10631,7 @@
         <v>4</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C696" t="s">
         <v>863</v>
@@ -10642,7 +10642,7 @@
         <v>4</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C697" t="s">
         <v>863</v>
@@ -10653,7 +10653,7 @@
         <v>4</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C698" t="s">
         <v>863</v>
@@ -10664,7 +10664,7 @@
         <v>4</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C699" t="s">
         <v>863</v>
@@ -10675,7 +10675,7 @@
         <v>4</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C700" t="s">
         <v>863</v>
@@ -10686,7 +10686,7 @@
         <v>4</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C701" t="s">
         <v>863</v>
@@ -10697,7 +10697,7 @@
         <v>4</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C702" t="s">
         <v>863</v>
@@ -10708,7 +10708,7 @@
         <v>4</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C703" t="s">
         <v>863</v>
@@ -10719,7 +10719,7 @@
         <v>4</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C704" t="s">
         <v>863</v>
@@ -10730,7 +10730,7 @@
         <v>4</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C705" t="s">
         <v>863</v>
@@ -10741,7 +10741,7 @@
         <v>4</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C706" t="s">
         <v>863</v>
@@ -10752,7 +10752,7 @@
         <v>4</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C707" t="s">
         <v>863</v>
@@ -10763,7 +10763,7 @@
         <v>4</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C708" t="s">
         <v>863</v>
@@ -10774,7 +10774,7 @@
         <v>4</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C709" t="s">
         <v>863</v>
@@ -10785,7 +10785,7 @@
         <v>4</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C710" t="s">
         <v>863</v>
@@ -10796,7 +10796,7 @@
         <v>4</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C711" t="s">
         <v>863</v>
@@ -10807,7 +10807,7 @@
         <v>4</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C712" t="s">
         <v>863</v>
@@ -10818,7 +10818,7 @@
         <v>4</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C713" t="s">
         <v>863</v>
@@ -10829,7 +10829,7 @@
         <v>4</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C714" t="s">
         <v>863</v>
@@ -10840,7 +10840,7 @@
         <v>4</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C715" t="s">
         <v>863</v>
@@ -10851,7 +10851,7 @@
         <v>4</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C716" t="s">
         <v>863</v>
@@ -10862,7 +10862,7 @@
         <v>4</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C717" t="s">
         <v>863</v>
@@ -10873,7 +10873,7 @@
         <v>4</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C718" t="s">
         <v>863</v>
@@ -10884,7 +10884,7 @@
         <v>4</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C719" t="s">
         <v>863</v>
@@ -10895,7 +10895,7 @@
         <v>4</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C720" t="s">
         <v>863</v>
@@ -10906,7 +10906,7 @@
         <v>4</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C721" t="s">
         <v>863</v>
@@ -10917,7 +10917,7 @@
         <v>4</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C722" t="s">
         <v>863</v>
@@ -10928,7 +10928,7 @@
         <v>4</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C723" t="s">
         <v>863</v>
@@ -10939,7 +10939,7 @@
         <v>4</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C724" t="s">
         <v>863</v>
@@ -10950,7 +10950,7 @@
         <v>4</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C725" t="s">
         <v>863</v>
@@ -10961,7 +10961,7 @@
         <v>4</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C726" t="s">
         <v>863</v>
@@ -10972,7 +10972,7 @@
         <v>4</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C727" t="s">
         <v>863</v>
@@ -10983,7 +10983,7 @@
         <v>4</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C728" t="s">
         <v>863</v>
@@ -10994,7 +10994,7 @@
         <v>4</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C729" t="s">
         <v>863</v>
@@ -11005,7 +11005,7 @@
         <v>4</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C730" t="s">
         <v>863</v>
@@ -11016,7 +11016,7 @@
         <v>4</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C731" t="s">
         <v>863</v>
@@ -11027,7 +11027,7 @@
         <v>4</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C732" t="s">
         <v>863</v>
@@ -11038,7 +11038,7 @@
         <v>4</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C733" t="s">
         <v>863</v>
@@ -11049,7 +11049,7 @@
         <v>4</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C734" t="s">
         <v>863</v>
@@ -11060,7 +11060,7 @@
         <v>4</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C735" t="s">
         <v>863</v>
@@ -11071,7 +11071,7 @@
         <v>4</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C736" t="s">
         <v>863</v>
@@ -11082,7 +11082,7 @@
         <v>4</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C737" t="s">
         <v>863</v>
@@ -11093,7 +11093,7 @@
         <v>4</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C738" t="s">
         <v>863</v>
@@ -11104,7 +11104,7 @@
         <v>4</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C739" t="s">
         <v>863</v>
@@ -11115,7 +11115,7 @@
         <v>4</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C740" t="s">
         <v>863</v>
@@ -11126,7 +11126,7 @@
         <v>4</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C741" t="s">
         <v>863</v>
@@ -11137,7 +11137,7 @@
         <v>4</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C742" t="s">
         <v>863</v>
@@ -11148,7 +11148,7 @@
         <v>4</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C743" t="s">
         <v>863</v>
@@ -11159,7 +11159,7 @@
         <v>4</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C744" t="s">
         <v>863</v>
@@ -11170,7 +11170,7 @@
         <v>4</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C745" t="s">
         <v>863</v>
@@ -11181,7 +11181,7 @@
         <v>4</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C746" t="s">
         <v>863</v>
@@ -11192,7 +11192,7 @@
         <v>4</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C747" t="s">
         <v>863</v>
@@ -11203,7 +11203,7 @@
         <v>4</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C748" t="s">
         <v>863</v>
@@ -11214,7 +11214,7 @@
         <v>4</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C749" t="s">
         <v>863</v>
@@ -11225,7 +11225,7 @@
         <v>4</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C750" t="s">
         <v>863</v>
@@ -11236,7 +11236,7 @@
         <v>4</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C751" t="s">
         <v>863</v>
@@ -11247,7 +11247,7 @@
         <v>4</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C752" t="s">
         <v>863</v>
@@ -11258,7 +11258,7 @@
         <v>4</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C753" t="s">
         <v>863</v>
@@ -11269,7 +11269,7 @@
         <v>4</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C754" t="s">
         <v>863</v>
@@ -11280,7 +11280,7 @@
         <v>4</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C755" t="s">
         <v>863</v>
@@ -11291,7 +11291,7 @@
         <v>4</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C756" t="s">
         <v>863</v>
@@ -11302,7 +11302,7 @@
         <v>4</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C757" t="s">
         <v>863</v>
@@ -11313,7 +11313,7 @@
         <v>4</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C758" t="s">
         <v>863</v>
@@ -11324,7 +11324,7 @@
         <v>4</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C759" t="s">
         <v>863</v>
@@ -11335,7 +11335,7 @@
         <v>4</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C760" t="s">
         <v>863</v>
@@ -11346,7 +11346,7 @@
         <v>4</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C761" t="s">
         <v>863</v>
@@ -11357,7 +11357,7 @@
         <v>4</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C762" t="s">
         <v>863</v>
@@ -11368,7 +11368,7 @@
         <v>4</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C763" t="s">
         <v>863</v>
@@ -11379,7 +11379,7 @@
         <v>4</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C764" t="s">
         <v>863</v>
@@ -11390,7 +11390,7 @@
         <v>4</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C765" t="s">
         <v>863</v>
@@ -11401,7 +11401,7 @@
         <v>4</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C766" t="s">
         <v>863</v>
@@ -11412,7 +11412,7 @@
         <v>4</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C767" t="s">
         <v>863</v>
@@ -11423,7 +11423,7 @@
         <v>4</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C768" t="s">
         <v>863</v>
@@ -11434,7 +11434,7 @@
         <v>4</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C769" t="s">
         <v>863</v>
@@ -11445,7 +11445,7 @@
         <v>4</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C770" t="s">
         <v>863</v>
@@ -11456,7 +11456,7 @@
         <v>4</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C771" t="s">
         <v>863</v>
@@ -11467,7 +11467,7 @@
         <v>4</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C772" t="s">
         <v>863</v>
@@ -11478,7 +11478,7 @@
         <v>4</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C773" t="s">
         <v>863</v>
@@ -11489,7 +11489,7 @@
         <v>4</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C774" t="s">
         <v>863</v>
@@ -11500,7 +11500,7 @@
         <v>4</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C775" t="s">
         <v>863</v>
@@ -11511,7 +11511,7 @@
         <v>4</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C776" t="s">
         <v>863</v>
@@ -11522,7 +11522,7 @@
         <v>4</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C777" t="s">
         <v>863</v>
@@ -11533,7 +11533,7 @@
         <v>4</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C778" t="s">
         <v>863</v>
@@ -11544,7 +11544,7 @@
         <v>4</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C779" t="s">
         <v>863</v>
@@ -11555,7 +11555,7 @@
         <v>4</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C780" t="s">
         <v>863</v>
@@ -11566,7 +11566,7 @@
         <v>4</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C781" t="s">
         <v>863</v>
@@ -11577,7 +11577,7 @@
         <v>4</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C782" t="s">
         <v>863</v>
@@ -11588,7 +11588,7 @@
         <v>4</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C783" t="s">
         <v>863</v>
@@ -11599,7 +11599,7 @@
         <v>4</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C784" t="s">
         <v>863</v>
@@ -11610,7 +11610,7 @@
         <v>4</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C785" t="s">
         <v>863</v>
@@ -11621,7 +11621,7 @@
         <v>4</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C786" t="s">
         <v>863</v>
@@ -11632,7 +11632,7 @@
         <v>4</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="C787" t="s">
         <v>863</v>
@@ -11643,7 +11643,7 @@
         <v>4</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C788" t="s">
         <v>863</v>
@@ -11654,7 +11654,7 @@
         <v>4</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C789" t="s">
         <v>863</v>
@@ -11665,7 +11665,7 @@
         <v>4</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="C790" t="s">
         <v>863</v>
@@ -11676,7 +11676,7 @@
         <v>4</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C791" t="s">
         <v>863</v>
@@ -11687,7 +11687,7 @@
         <v>4</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C792" t="s">
         <v>863</v>
@@ -11698,7 +11698,7 @@
         <v>4</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C793" t="s">
         <v>863</v>
@@ -11709,7 +11709,7 @@
         <v>4</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C794" t="s">
         <v>863</v>
@@ -11720,7 +11720,7 @@
         <v>4</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C795" t="s">
         <v>863</v>
@@ -11731,7 +11731,7 @@
         <v>4</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C796" t="s">
         <v>863</v>
@@ -11742,7 +11742,7 @@
         <v>4</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C797" t="s">
         <v>863</v>
@@ -11753,7 +11753,7 @@
         <v>4</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C798" t="s">
         <v>863</v>
@@ -11764,7 +11764,7 @@
         <v>4</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C799" t="s">
         <v>863</v>
@@ -11775,7 +11775,7 @@
         <v>4</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C800" t="s">
         <v>863</v>
@@ -11786,7 +11786,7 @@
         <v>4</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C801" t="s">
         <v>863</v>
@@ -11797,7 +11797,7 @@
         <v>4</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C802" t="s">
         <v>863</v>
@@ -11808,7 +11808,7 @@
         <v>4</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C803" t="s">
         <v>863</v>
@@ -11819,7 +11819,7 @@
         <v>4</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C804" t="s">
         <v>863</v>
@@ -11830,7 +11830,7 @@
         <v>4</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C805" t="s">
         <v>863</v>
@@ -11841,7 +11841,7 @@
         <v>4</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C806" t="s">
         <v>863</v>
@@ -11852,7 +11852,7 @@
         <v>4</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C807" t="s">
         <v>863</v>
@@ -11863,7 +11863,7 @@
         <v>4</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C808" t="s">
         <v>863</v>
@@ -11874,7 +11874,7 @@
         <v>4</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C809" t="s">
         <v>863</v>
@@ -11885,7 +11885,7 @@
         <v>4</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C810" t="s">
         <v>863</v>
@@ -11896,7 +11896,7 @@
         <v>4</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C811" t="s">
         <v>863</v>
@@ -11907,7 +11907,7 @@
         <v>4</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C812" t="s">
         <v>863</v>
@@ -11918,7 +11918,7 @@
         <v>4</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C813" t="s">
         <v>863</v>
@@ -11929,7 +11929,7 @@
         <v>4</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C814" t="s">
         <v>863</v>
@@ -11940,7 +11940,7 @@
         <v>4</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C815" t="s">
         <v>863</v>
@@ -11951,7 +11951,7 @@
         <v>4</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C816" t="s">
         <v>863</v>
@@ -11962,7 +11962,7 @@
         <v>4</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C817" t="s">
         <v>863</v>
@@ -11973,7 +11973,7 @@
         <v>4</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C818" t="s">
         <v>863</v>
@@ -11984,7 +11984,7 @@
         <v>4</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C819" t="s">
         <v>863</v>
@@ -11995,7 +11995,7 @@
         <v>4</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C820" t="s">
         <v>863</v>
@@ -12006,7 +12006,7 @@
         <v>4</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C821" t="s">
         <v>863</v>
@@ -12017,7 +12017,7 @@
         <v>4</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C822" t="s">
         <v>863</v>
@@ -12028,7 +12028,7 @@
         <v>4</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C823" t="s">
         <v>863</v>
@@ -12039,7 +12039,7 @@
         <v>4</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C824" t="s">
         <v>863</v>
@@ -12050,7 +12050,7 @@
         <v>4</v>
       </c>
       <c r="B825" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C825" t="s">
         <v>863</v>
@@ -12061,7 +12061,7 @@
         <v>4</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C826" t="s">
         <v>863</v>
@@ -12072,7 +12072,7 @@
         <v>4</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C827" t="s">
         <v>863</v>
@@ -12083,7 +12083,7 @@
         <v>4</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C828" t="s">
         <v>863</v>
@@ -12094,7 +12094,7 @@
         <v>4</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C829" t="s">
         <v>863</v>
@@ -12105,7 +12105,7 @@
         <v>4</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C830" t="s">
         <v>863</v>
@@ -12116,7 +12116,7 @@
         <v>4</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C831" t="s">
         <v>863</v>
@@ -12127,7 +12127,7 @@
         <v>4</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C832" t="s">
         <v>863</v>
@@ -12138,7 +12138,7 @@
         <v>4</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C833" t="s">
         <v>863</v>
@@ -12149,7 +12149,7 @@
         <v>4</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C834" t="s">
         <v>863</v>
@@ -12160,7 +12160,7 @@
         <v>4</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C835" t="s">
         <v>863</v>
@@ -12171,7 +12171,7 @@
         <v>4</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C836" t="s">
         <v>863</v>
@@ -12182,7 +12182,7 @@
         <v>4</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C837" t="s">
         <v>863</v>
@@ -12193,7 +12193,7 @@
         <v>4</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C838" t="s">
         <v>863</v>
@@ -12204,7 +12204,7 @@
         <v>4</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C839" t="s">
         <v>863</v>
@@ -12215,7 +12215,7 @@
         <v>4</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C840" t="s">
         <v>863</v>
@@ -12226,7 +12226,7 @@
         <v>4</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C841" t="s">
         <v>863</v>
@@ -12237,7 +12237,7 @@
         <v>4</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C842" t="s">
         <v>863</v>
@@ -12248,7 +12248,7 @@
         <v>4</v>
       </c>
       <c r="B843" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C843" t="s">
         <v>863</v>
@@ -12259,7 +12259,7 @@
         <v>4</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C844" t="s">
         <v>863</v>
@@ -12270,7 +12270,7 @@
         <v>4</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C845" t="s">
         <v>863</v>
@@ -12281,7 +12281,7 @@
         <v>4</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C846" t="s">
         <v>863</v>
@@ -12292,7 +12292,7 @@
         <v>4</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C847" t="s">
         <v>863</v>
@@ -12303,7 +12303,7 @@
         <v>4</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C848" t="s">
         <v>863</v>
@@ -12314,7 +12314,7 @@
         <v>4</v>
       </c>
       <c r="B849" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C849" t="s">
         <v>863</v>
@@ -12325,7 +12325,7 @@
         <v>4</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C850" t="s">
         <v>863</v>
@@ -12336,7 +12336,7 @@
         <v>4</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C851" t="s">
         <v>863</v>
@@ -12347,7 +12347,7 @@
         <v>4</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C852" t="s">
         <v>863</v>
@@ -12358,7 +12358,7 @@
         <v>4</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C853" t="s">
         <v>863</v>
@@ -12369,7 +12369,7 @@
         <v>4</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C854" t="s">
         <v>863</v>
@@ -12380,7 +12380,7 @@
         <v>4</v>
       </c>
       <c r="B855" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C855" t="s">
         <v>863</v>
@@ -12391,7 +12391,7 @@
         <v>4</v>
       </c>
       <c r="B856" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C856" t="s">
         <v>863</v>
@@ -12402,7 +12402,7 @@
         <v>4</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C857" t="s">
         <v>863</v>
@@ -12413,7 +12413,7 @@
         <v>4</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C858" t="s">
         <v>863</v>
@@ -12424,7 +12424,7 @@
         <v>4</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C859" t="s">
         <v>863</v>
@@ -12435,7 +12435,7 @@
         <v>4</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C860" t="s">
         <v>863</v>
@@ -12446,7 +12446,7 @@
         <v>4</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C861" t="s">
         <v>863</v>
@@ -12457,7 +12457,7 @@
         <v>4</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C862" t="s">
         <v>863</v>
@@ -12468,7 +12468,7 @@
         <v>4</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C863" t="s">
         <v>863</v>
@@ -12479,7 +12479,7 @@
         <v>4</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C864" t="s">
         <v>863</v>
@@ -12490,7 +12490,7 @@
         <v>4</v>
       </c>
       <c r="B865" s="2" t="s">
-        <v>869</v>
+        <v>862</v>
       </c>
       <c r="C865" t="s">
         <v>863</v>
@@ -12498,9 +12498,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D865">
-    <sortState ref="A2:E867">
-      <sortCondition ref="A2:A867"/>
-      <sortCondition ref="B2:B867"/>
+    <sortState ref="A2:D865">
+      <sortCondition ref="A2:A865"/>
+      <sortCondition ref="B2:B865"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>